<commit_message>
Update Code Systems.xlsx - HCPCS details tbd when loader is written
</commit_message>
<xml_diff>
--- a/codevalidator-api/docs/Code Systems.xlsx
+++ b/codevalidator-api/docs/Code Systems.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ai-vmdc1\RedirectedFolders\amore\Desktop\SITE_VSAC\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A7914A2A-34DB-4204-9999-F6C1694A1D9C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7080" tabRatio="986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>Code System</t>
   </si>
@@ -95,9 +101,6 @@
     <t>fixed length</t>
   </si>
   <si>
-    <t>LONGUF.txt, MEDU.txt, SHORTU.txt</t>
-  </si>
-  <si>
     <t>Position 1 to 9</t>
   </si>
   <si>
@@ -113,9 +116,6 @@
     <t>ICD9CM_DX</t>
   </si>
   <si>
-    <t>CMS32_DESC_LONG_DX.txt, CMS32_DESC_SHORT_DX.txt</t>
-  </si>
-  <si>
     <t>Position 1 to 5</t>
   </si>
   <si>
@@ -146,9 +146,6 @@
     <t>ICD10CM</t>
   </si>
   <si>
-    <t>icd10cm_order_2015.txt</t>
-  </si>
-  <si>
     <t>Position 7 to 14</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>ICD10PCS</t>
   </si>
   <si>
-    <t>icd10pcs_order_2015.txt</t>
-  </si>
-  <si>
     <t>LOINC</t>
   </si>
   <si>
@@ -215,19 +209,37 @@
     <t>SNOMED-CT</t>
   </si>
   <si>
-    <t>sct2_Description_Full-en_US1000124_20150901.txt</t>
-  </si>
-  <si>
     <t>Tab 5 (CONCEPT ID)</t>
   </si>
   <si>
     <t>Tab 6 (Language Code)</t>
+  </si>
+  <si>
+    <t>LONGULT.txt, MEDU.txt, SHORTU.txt</t>
+  </si>
+  <si>
+    <t>CMS32_DESC_LONG_SHORT_DX.txt</t>
+  </si>
+  <si>
+    <t>icd10cm_order_2017.txt</t>
+  </si>
+  <si>
+    <t>icd10pcs_order_2017.txt</t>
+  </si>
+  <si>
+    <t>sct2_Description_Snapshot-en_US1000124_20170901.txt</t>
+  </si>
+  <si>
+    <t>HCPCS</t>
+  </si>
+  <si>
+    <t>HCPC2018_CONTR_ANWEB.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -294,6 +306,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -341,7 +356,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -374,9 +389,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -409,6 +441,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -584,11 +633,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -670,27 +719,27 @@
         <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
@@ -699,56 +748,56 @@
         <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>
@@ -757,27 +806,27 @@
         <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -786,106 +835,120 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>